<commit_message>
working on adding to spent column
</commit_message>
<xml_diff>
--- a/expense_tracker.xlsx
+++ b/expense_tracker.xlsx
@@ -351,7 +351,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="20"/>
   </cols>
@@ -391,7 +391,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01/09/19</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -413,11 +413,16 @@
           <t>Gas</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C3" t="n">
         <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>168.71</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <f>(C2:C7 - D2:D7)</f>
@@ -430,6 +435,11 @@
           <t>Groceries</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C4" t="n">
         <v>200</v>
       </c>
@@ -449,6 +459,11 @@
           <t>Restaurants</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>0</t>
@@ -470,6 +485,11 @@
           <t>Savings</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>0</t>
@@ -489,6 +509,11 @@
       <c r="A7" t="inlineStr">
         <is>
           <t>Recreation</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">

</xml_diff>

<commit_message>
functioning addition of values
</commit_message>
<xml_diff>
--- a/expense_tracker.xlsx
+++ b/expense_tracker.xlsx
@@ -351,7 +351,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="20"/>
   </cols>
@@ -422,7 +422,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <f>(C2:C7 - D2:D7)</f>

</xml_diff>

<commit_message>
submits value to correct category
</commit_message>
<xml_diff>
--- a/expense_tracker.xlsx
+++ b/expense_tracker.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,20 +364,15 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Budgeted</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Budgeted</t>
+          <t>Spent</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>Spent</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>Remaining</t>
         </is>
@@ -389,21 +384,14 @@
           <t>Rent</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>900</v>
       </c>
       <c r="C2" t="n">
-        <v>900</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E2">
-        <f>(C2:C7 - D2:D7)</f>
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>
@@ -413,19 +401,14 @@
           <t>Gas</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>200</v>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
-      </c>
-      <c r="D3" t="n">
-        <v>30</v>
-      </c>
-      <c r="E3">
-        <f>(C2:C7 - D2:D7)</f>
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>
@@ -435,21 +418,16 @@
           <t>Groceries</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" t="n">
         <v>200</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4">
-        <f>(C2:C7 - D2:D7)</f>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>
@@ -469,13 +447,8 @@
           <t>0</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E5">
-        <f>(C2:C7 - D2:D7)</f>
+      <c r="D5">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>
@@ -495,13 +468,8 @@
           <t>0</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E6">
-        <f>(C2:C7 - D2:D7)</f>
+      <c r="D6">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>
@@ -521,13 +489,8 @@
           <t>0</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E7">
-        <f>(C2:C7 - D2:D7)</f>
+      <c r="D7">
+        <f>(B2:B7 - C2:C7)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
everything works except for scheduling
</commit_message>
<xml_diff>
--- a/expense_tracker.xlsx
+++ b/expense_tracker.xlsx
@@ -354,6 +354,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="20"/>
+    <col customWidth="1" max="2" min="2" width="17"/>
+    <col customWidth="1" max="4" min="4" width="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -364,17 +366,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Budgeted</t>
+          <t>Budgeted ($)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Spent</t>
+          <t>Spent ($)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Remaining</t>
+          <t>Remaining ($)</t>
         </is>
       </c>
     </row>
@@ -387,8 +389,10 @@
       <c r="B2" t="n">
         <v>900</v>
       </c>
-      <c r="C2" t="n">
-        <v>26</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="D2">
         <f>(B2:B7 - C2:C7)</f>
@@ -404,8 +408,10 @@
       <c r="B3" t="n">
         <v>200</v>
       </c>
-      <c r="C3" t="n">
-        <v>43</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="D3">
         <f>(B2:B7 - C2:C7)</f>
@@ -437,10 +443,8 @@
           <t>Restaurants</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B5" t="n">
+        <v>100</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -458,10 +462,8 @@
           <t>Savings</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>500</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -479,15 +481,11 @@
           <t>Recreation</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
       </c>
       <c r="D7">
         <f>(B2:B7 - C2:C7)</f>

</xml_diff>